<commit_message>
rebuild feed, think to make interface to feed builder
</commit_message>
<xml_diff>
--- a/nodejs/feedBuilder/data.xlsx
+++ b/nodejs/feedBuilder/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="shop" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="109">
   <si>
     <t>name</t>
   </si>
@@ -351,6 +351,76 @@
   </si>
   <si>
     <t>https://erabeauty.ru/wp-content/uploads/2025/03/era-logo.svg</t>
+  </si>
+  <si>
+    <t>https://erabeauty.ru/team/opanashchuk_marina_nikolaevna/</t>
+  </si>
+  <si>
+    <t>Опанащук Марина Николаевна</t>
+  </si>
+  <si>
+    <t>Врач-дерматовенеролог, врач-косметолог</t>
+  </si>
+  <si>
+    <t>https://erabeauty.ru/wp-content/uploads/2025/04/photo_2025-04-17_14-40-57-768x1024.jpg</t>
+  </si>
+  <si>
+    <t>https://erabeauty.ru/team/chernyshova_mariya_mihajlovna/</t>
+  </si>
+  <si>
+    <t>Чернышова Мария Михайловна</t>
+  </si>
+  <si>
+    <t>https://erabeauty.ru/wp-content/uploads/2025/04/photo_2025-04-17_14-41-00-768x1024.jpg</t>
+  </si>
+  <si>
+    <t>https://erabeauty.ru/team/serikova_tatyana_leonidovna/</t>
+  </si>
+  <si>
+    <t>Серикова Татьяна Леонидовна</t>
+  </si>
+  <si>
+    <t>Медицинская сестра по косметологии, косметолог-эстетист, косметолог-подолог</t>
+  </si>
+  <si>
+    <t>https://erabeauty.ru/wp-content/uploads/2025/04/серикова_татьяна-1-806x1024.jpg</t>
+  </si>
+  <si>
+    <t>9 (473) 211-20-28</t>
+  </si>
+  <si>
+    <t>10 (473) 211-20-28</t>
+  </si>
+  <si>
+    <t>11 (473) 211-20-28</t>
+  </si>
+  <si>
+    <t>ул. Московский проспект 34</t>
+  </si>
+  <si>
+    <t>ул. Московский проспект 35</t>
+  </si>
+  <si>
+    <t>ул. Московский проспект 36</t>
+  </si>
+  <si>
+    <t>ГОУ ВПО «ВГМУ им. Н.Н. Бурденко»; 2022; Базовое образование; Лечебное дело, врач||
+ФГБОУ ВО ТГУ им. Г.Р. Державина; 2024; ординатура по специальности «Дерматовенерология»; Дерматовенерология||
+ЧУД ПО «Институт профессиональных технологий и сервиса ФиЗ»; 2024; сертификат специалиста по специальности «Косметология»;Косметология</t>
+  </si>
+  <si>
+    <t>ГОУ СПО «Северодвинское медицинское училище»; 1993; Базовое образование; Медицинская сестра||
+Международный Учебный Центр «Формула красоты»; 2008; специальность «косметолог-эстетист»; ||
+компания Studex; 2010; курс по технике прокола ушей; Косметология ||
+ООО «Межрегиональный центр непрерывного медицинского и фармацевтического образования»; 2020; Сестринское дело в косметологии; Косметология ||
+ООО «Межрегиональный центр непрерывного медицинского и фармацевтического образования»; 2020; сертификат специалиста по специальности «Сестринское дело в косметологии»;Косметлогия ||
+Школа подологии «Мирада» (г. Санкт-Петербург); 2020; косметолог-подолог;Косметология</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГОУ ВПО «ВГМУ им. Н.Н. Бурденко»;2021;Базовое образование;Лечебное дело, врач||
+ГОУ ВПО «ВГМУ им. Н.Н. Бурденко»;2024; ординатура по специальности «Дерматовенерология»;Дерматовенерология||
+ГОУ ВПО «ВГМУ им. Н.Н. Бурденко»;2024; сертификат специалиста по специальности «Косметология»;Косметология||
+</t>
   </si>
 </sst>
 </file>
@@ -720,20 +790,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +816,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -763,7 +833,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -780,7 +850,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -791,7 +861,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -802,7 +872,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -813,7 +883,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -824,22 +894,22 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -848,30 +918,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" customWidth="1"/>
-    <col min="3" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="16" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +991,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -968,7 +1038,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1085,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1062,7 +1132,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1179,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1156,7 +1226,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1203,7 +1273,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1250,7 +1320,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1297,7 +1367,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1344,7 +1414,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1391,7 +1461,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1436,6 +1506,138 @@
       </c>
       <c r="Q12" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" t="s">
+        <v>100</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" t="s">
+        <v>101</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15">
+        <v>15</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" t="s">
+        <v>102</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>